<commit_message>
Updated README and requirement.txt
</commit_message>
<xml_diff>
--- a/human_facts.xlsx
+++ b/human_facts.xlsx
@@ -1,37 +1,103 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANTARA DAS\Documents\GitDemo\SDGP\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD119EB-9128-4671-9EAA-09F58838AF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Fact Number</t>
+  </si>
+  <si>
+    <t>One-Liner Human Fact</t>
+  </si>
+  <si>
+    <t>Generated Article</t>
+  </si>
+  <si>
+    <t>We walk on four legs, with feet that sway,
+And breathe oxygen, every single day!</t>
+  </si>
+  <si>
+    <t>**The Amazing Animals of Our World: Walking and Breathe**
+Have you ever stopped to think about the incredible creatures that roam our planet? From the tiniest insects to the mightiest mammals, each species has evolved unique physical characteristics that enable them to survive and thrive in their environments.
+Let's take a closer look at some fascinating animals that exhibit remarkable features like four legs and breathing oxygen every day.
+**The Walking Machine**
+Most of us are familiar with humans as bipedal creatures. Our legs allow us to walk upright on two feet, which is essential for locomotion and social interaction. But did you know that many other animals also possess four legs? For example:
+* Dogs: With their sturdy legs and powerful muscles, dogs can run at speeds of up to 45 miles per hour.
+* Cats: Despite their slender bodies, cats are agile and fast, with some species able to climb trees or chase prey with incredible speed.
+* Bears: These omnivores use their four legs to move through dense forests or cross rivers with ease.
+But what about the animals that don't walk on two feet? Well, let's take a look at some of the creatures that breathe oxygen every day:
+**The Oxygen Bathers**
+Some species of fish and other aquatic animals are able to extract oxygen from water using specialized organs called gills. This allows them to survive underwater for extended periods without surfacing for air.
+* Goldfish: These tiny fish can absorb oxygen from the water using their gills, allowing them to thrive in cold, polluted waters.
+* Sharks: Despite their fearsome reputation, sharks are actually filter feeders that use their gills to extract oxygen from the water.
+**The Breathe-Oxygen Machines**
+Some animals have evolved remarkable adaptations that enable them to breathe oxygen every day. For example:
+* Flying squirrels: These nocturnal creatures use a combination of flapping their arms and using stored oxygen in their muscles to stay aloft for hours at a time.
+* Penguins: While they may not be as well-known for their swimming abilities, penguins are able to dive deep into the ocean and then surface with stored oxygen in their bodies.
+**The Oxygen Recycling Machines**
+Finally, some animals have evolved clever mechanisms that allow them to recycle oxygen from their surroundings. For example:
+* Elephants: These gentle giants use a specialized network of blood vessels called the "circulatory tree" to transport oxygen-rich blood throughout their body.
+* Dolphins: As intelligent and social creatures, dolphins are able to recognize individual members of their pod and even communicate with each other using complex vocalizations that involve oxygen-rich gases.
+These incredible animals remind us of just how amazing and diverse life on Earth is. From the tiniest insects to the mightiest mammals, every species has evolved unique features that enable them to survive and thrive in their environments.</t>
+  </si>
+  <si>
+    <t>Humans have a brain that's quite fine, it processes thoughts and feelings so divine.</t>
+  </si>
+  <si>
+    <t>**The Marvelous Human Brain: A Complex and Divine Organ**
+The human brain is often referred to as the most complex and intricate organ in the human body. Composed of billions of neurons, glial cells, and other supporting tissue, this incredible structure is capable of processing thoughts, feelings, and experiences with unprecedented precision.
+At its core, the brain's primary function is to facilitate consciousness, enabling us to think, learn, and experience the world around us. This remarkable ability to process information is made possible by the intricate interplay between neurons, which transmit and receive electrical signals that allow our brains to perform a wide range of cognitive tasks.
+**Processing Thoughts: The Cognitive Machine**
+The brain's neural networks are responsible for processing thoughts and feelings, allowing us to form connections between seemingly unrelated ideas. This complex process involves multiple stages, including perception, attention, memory consolidation, and decision-making. Each stage is fueled by the coordinated activity of billions of neurons, which communicate with each other through electrical and chemical signals.
+**Emotional Intelligence: The Brain's Emotional Center**
+The brain also has an emotional center, known as the amygdala, which plays a crucial role in processing emotions such as fear, anxiety, and happiness. This complex network allows us to experience a wide range of emotions and respond accordingly, enabling us to interact with our environment in a meaningful way.
+**Learning and Memory: The Brain's Adaptation Machine**
+The brain is constantly learning and adapting throughout our lives, allowing us to develop new skills and abilities. Through a process called synaptic plasticity, the connections between neurons can be strengthened or weakened based on experience, enabling us to refine our thoughts and behaviors over time.
+**The Impact of Brain Function on Human Experience**
+Understanding the human brain's incredible capabilities is not just fascinating; it also has significant implications for various fields such as psychology, neuroscience, education, and healthcare. By studying the intricacies of brain function, researchers can gain insights into the development of new treatments for mental health disorders, improve learning outcomes in education, and develop more effective training programs.
+**Conclusion**
+In conclusion, the human brain is a remarkable organ that has evolved to become an incredibly complex system capable of processing thoughts, feelings, and experiences with precision. By exploring its intricate workings, we can gain a deeper understanding of the incredible abilities of this biological marvel and appreciate the importance of brain function in shaping our lives and experiences.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +112,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,49 +436,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.6328125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Fact Number</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>One-Liner Human Fact</t>
-        </is>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Humans are bipedal, meaning they walk on two legs with ease!</t>
-        </is>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Humans are born with around 300 bones, yet only 206 are present at birth!</t>
-        </is>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>